<commit_message>
emailing timer should work
</commit_message>
<xml_diff>
--- a/FutureYou/ATB/ATB 27-02-2025.xlsx
+++ b/FutureYou/ATB/ATB 27-02-2025.xlsx
@@ -63,7 +63,7 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="2"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -72,9 +72,6 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="2"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -514,22 +511,22 @@
           <t>Contact</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>Invoice Date</t>
         </is>
       </c>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>Ageing Days</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="G2" s="1" t="inlineStr">
         <is>
           <t>Due Date</t>
         </is>
       </c>
-      <c r="H2" s="3" t="inlineStr">
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t>Overdue Days</t>
         </is>
@@ -554,12 +551,12 @@
           <t>Category</t>
         </is>
       </c>
-      <c r="M2" s="6" t="inlineStr">
+      <c r="M2" s="1" t="inlineStr">
         <is>
           <t>Consultant</t>
         </is>
       </c>
-      <c r="N2" s="6" t="inlineStr">
+      <c r="N2" s="1" t="inlineStr">
         <is>
           <t>Comments</t>
         </is>

</xml_diff>